<commit_message>
Modificados parametros de las querys de pagos y facturas
</commit_message>
<xml_diff>
--- a/templates/report/pagos.xlsx
+++ b/templates/report/pagos.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://manpowergroupapps-my.sharepoint.com/personal/cesar_ramos_ciberexperis_es/Documents/Documents/Cotown/git/cotown-back/templates/report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="71" documentId="13_ncr:1_{E16B1738-8929-454F-8CD4-B6BA4B1CC6A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{15421EC2-663F-4869-B0F5-36B97E3BDB9C}"/>
+  <xr:revisionPtr revIDLastSave="72" documentId="13_ncr:1_{E16B1738-8929-454F-8CD4-B6BA4B1CC6A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{31FF3F9C-B54F-4C7A-8CE2-A9770E610D01}"/>
   <bookViews>
-    <workbookView xWindow="1875" yWindow="1845" windowWidth="25875" windowHeight="11115" tabRatio="750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" tabRatio="750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Paises" sheetId="41" r:id="rId1"/>
+    <sheet name="Pagos" sheetId="41" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -199,7 +199,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -219,7 +219,6 @@
     </xf>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hipervínculo 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -705,7 +704,6 @@
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="10"/>
-      <c r="D3" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -714,6 +712,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="220d4249-f262-4642-a86b-ff46de6e315d">
@@ -722,15 +729,6 @@
     <TaxCatchAll xmlns="965e701d-44ad-4371-a199-8fefe953808c"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -931,20 +929,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91323775-37AE-44DC-8259-7FCDE5D849E0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC650EC1-3E41-4FC6-BA6C-52921951A8DA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="220d4249-f262-4642-a86b-ff46de6e315d"/>
     <ds:schemaRef ds:uri="965e701d-44ad-4371-a199-8fefe953808c"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91323775-37AE-44DC-8259-7FCDE5D849E0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Añadidos campos al informe de pagos
</commit_message>
<xml_diff>
--- a/templates/report/pagos.xlsx
+++ b/templates/report/pagos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://manpowergroupapps-my.sharepoint.com/personal/cesar_ramos_ciberexperis_es/Documents/Documents/Cotown/git/cotown-back/templates/report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="76" documentId="13_ncr:1_{E16B1738-8929-454F-8CD4-B6BA4B1CC6A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{52BE1261-0534-486C-B5E7-FE8934382FBA}"/>
+  <xr:revisionPtr revIDLastSave="84" documentId="13_ncr:1_{E16B1738-8929-454F-8CD4-B6BA4B1CC6A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{81CD14C7-A585-485F-86A3-704352D06EFE}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4755" yWindow="-16320" windowWidth="38640" windowHeight="15840" tabRatio="750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pagos" sheetId="41" r:id="rId1"/>
@@ -47,9 +47,6 @@
     <t>id</t>
   </si>
   <si>
-    <t>Payment_id</t>
-  </si>
-  <si>
     <t>Fecha de abono</t>
   </si>
   <si>
@@ -59,9 +56,6 @@
     <t>Payment_type</t>
   </si>
   <si>
-    <t>Payment_method</t>
-  </si>
-  <si>
     <t>Amount</t>
   </si>
   <si>
@@ -71,37 +65,43 @@
     <t>Concepto del pago</t>
   </si>
   <si>
-    <t>Payment_concept</t>
-  </si>
-  <si>
-    <t>Customer_name</t>
-  </si>
-  <si>
-    <t>Resource_type</t>
-  </si>
-  <si>
     <t>Tipo de recurso</t>
   </si>
   <si>
     <t>Código de recurso</t>
   </si>
   <si>
-    <t>Resource_code</t>
-  </si>
-  <si>
     <t>Dirección del recurso</t>
   </si>
   <si>
-    <t>Resource_address</t>
-  </si>
-  <si>
     <t>Proveedor del recurso</t>
   </si>
   <si>
     <t>Issued_date</t>
   </si>
   <si>
-    <t>Resource_provider_name</t>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Payment_method.Name</t>
+  </si>
+  <si>
+    <t>Concept</t>
+  </si>
+  <si>
+    <t>Customer.Name</t>
+  </si>
+  <si>
+    <t>Booking.Resource.Resource_type</t>
+  </si>
+  <si>
+    <t>Booking.Resource.Code</t>
+  </si>
+  <si>
+    <t>Booking.Resource.Address</t>
+  </si>
+  <si>
+    <t>Booking.Resource.Provider.Name</t>
   </si>
 </sst>
 </file>
@@ -616,7 +616,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -639,66 +639,66 @@
         <v>3</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>6</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
Cambios en el informe de pagos
</commit_message>
<xml_diff>
--- a/templates/report/pagos.xlsx
+++ b/templates/report/pagos.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\Development\projects\ciber\cotown\back\templates\report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://manpowergroupapps-my.sharepoint.com/personal/cesar_ramos_ciberexperis_es/Documents/Documents/Cotown/git/cotown-back/templates/report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8156F13E-1658-4ED8-A134-CC8A1A507743}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{8156F13E-1658-4ED8-A134-CC8A1A507743}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{32CD715D-1DD8-4398-9BB2-CE926B91D449}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="345" yWindow="3075" windowWidth="28470" windowHeight="11385" tabRatio="750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pagos" sheetId="41" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>.</t>
   </si>
@@ -72,6 +72,12 @@
   </si>
   <si>
     <t>Pagos</t>
+  </si>
+  <si>
+    <t>Fecha de checkin</t>
+  </si>
+  <si>
+    <t>Fecha de checkout</t>
   </si>
 </sst>
 </file>
@@ -568,9 +574,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F48469C1-5DA9-43F7-A0B7-76DC91FAD532}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -580,19 +588,19 @@
     <col min="5" max="5" width="22.140625" style="5" customWidth="1"/>
     <col min="6" max="6" width="36.28515625" style="1" customWidth="1"/>
     <col min="7" max="7" width="29.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="21.42578125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="20.42578125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="26.42578125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="23.7109375" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="11.42578125" style="1"/>
+    <col min="8" max="10" width="21.42578125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="20.42578125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="26.42578125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="23.7109375" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -618,16 +626,22 @@
         <v>8</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -641,6 +655,8 @@
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -649,6 +665,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="220d4249-f262-4642-a86b-ff46de6e315d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="965e701d-44ad-4371-a199-8fefe953808c"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101001BDC921D6C313740BA67D7760DC75571" ma:contentTypeVersion="9" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="ec6cd274e87ab0abf30bec2e834aaf15">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="220d4249-f262-4642-a86b-ff46de6e315d" xmlns:ns3="965e701d-44ad-4371-a199-8fefe953808c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0e77808c4f084d99d477d3de919e85b9" ns2:_="" ns3:_="">
     <xsd:import namespace="220d4249-f262-4642-a86b-ff46de6e315d"/>
@@ -845,27 +881,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC650EC1-3E41-4FC6-BA6C-52921951A8DA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="220d4249-f262-4642-a86b-ff46de6e315d"/>
+    <ds:schemaRef ds:uri="965e701d-44ad-4371-a199-8fefe953808c"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="220d4249-f262-4642-a86b-ff46de6e315d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="965e701d-44ad-4371-a199-8fefe953808c"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91323775-37AE-44DC-8259-7FCDE5D849E0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2190EF49-E186-4D77-87E3-BC317999ED9E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -882,23 +917,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91323775-37AE-44DC-8259-7FCDE5D849E0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC650EC1-3E41-4FC6-BA6C-52921951A8DA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="220d4249-f262-4642-a86b-ff46de6e315d"/>
-    <ds:schemaRef ds:uri="965e701d-44ad-4371-a199-8fefe953808c"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Modificaciones en el informe de pagos
</commit_message>
<xml_diff>
--- a/templates/report/pagos.xlsx
+++ b/templates/report/pagos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://manpowergroupapps-my.sharepoint.com/personal/cesar_ramos_ciberexperis_es/Documents/Documents/Cotown/git/cotown-back/templates/report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{8156F13E-1658-4ED8-A134-CC8A1A507743}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54E14CD2-E12E-406F-B056-FA9807B963B1}"/>
+  <xr:revisionPtr revIDLastSave="56" documentId="13_ncr:1_{8156F13E-1658-4ED8-A134-CC8A1A507743}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{04621FAD-930B-4028-831A-47F191BDCBBF}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8205" yWindow="-15885" windowWidth="21240" windowHeight="12810" tabRatio="750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pagos" sheetId="41" r:id="rId1"/>
@@ -35,21 +35,12 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
-    <t>.</t>
-  </si>
-  <si>
     <t>Importe</t>
   </si>
   <si>
     <t>Cliente</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>Fecha de abono</t>
-  </si>
-  <si>
     <t>Tipo de pago</t>
   </si>
   <si>
@@ -68,9 +59,6 @@
     <t>Dirección del recurso</t>
   </si>
   <si>
-    <t>Proveedor del recurso</t>
-  </si>
-  <si>
     <t>Pagos</t>
   </si>
   <si>
@@ -81,6 +69,18 @@
   </si>
   <si>
     <t>Fecha de pago</t>
+  </si>
+  <si>
+    <t>Código</t>
+  </si>
+  <si>
+    <t>Nombre del proveedor</t>
+  </si>
+  <si>
+    <t>Id reserva</t>
+  </si>
+  <si>
+    <t>Fecha de emisión</t>
   </si>
 </sst>
 </file>
@@ -175,9 +175,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
@@ -191,6 +188,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -580,85 +580,87 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F48469C1-5DA9-43F7-A0B7-76DC91FAD532}">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.140625" style="1" customWidth="1"/>
-    <col min="2" max="3" width="24.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="8" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" style="8" customWidth="1"/>
-    <col min="6" max="6" width="22.140625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="36.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="29.28515625" style="1" customWidth="1"/>
-    <col min="9" max="11" width="21.42578125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="20.42578125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="26.42578125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="23.7109375" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="19.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="46.140625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="45" style="7" customWidth="1"/>
+    <col min="5" max="5" width="19" style="4" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="22.140625" style="1" customWidth="1"/>
+    <col min="8" max="9" width="21.42578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="37.5703125" style="1" customWidth="1"/>
+    <col min="11" max="13" width="21.42578125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="20.42578125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="26.42578125" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="C2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>0</v>
-      </c>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
       <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
+      <c r="C3" s="9"/>
       <c r="D3" s="10"/>
-      <c r="E3" s="11"/>
+      <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -668,6 +670,7 @@
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -676,6 +679,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="220d4249-f262-4642-a86b-ff46de6e315d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="965e701d-44ad-4371-a199-8fefe953808c"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101001BDC921D6C313740BA67D7760DC75571" ma:contentTypeVersion="9" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="ec6cd274e87ab0abf30bec2e834aaf15">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="220d4249-f262-4642-a86b-ff46de6e315d" xmlns:ns3="965e701d-44ad-4371-a199-8fefe953808c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0e77808c4f084d99d477d3de919e85b9" ns2:_="" ns3:_="">
     <xsd:import namespace="220d4249-f262-4642-a86b-ff46de6e315d"/>
@@ -872,27 +895,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC650EC1-3E41-4FC6-BA6C-52921951A8DA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="220d4249-f262-4642-a86b-ff46de6e315d"/>
+    <ds:schemaRef ds:uri="965e701d-44ad-4371-a199-8fefe953808c"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="220d4249-f262-4642-a86b-ff46de6e315d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="965e701d-44ad-4371-a199-8fefe953808c"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91323775-37AE-44DC-8259-7FCDE5D849E0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2190EF49-E186-4D77-87E3-BC317999ED9E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -909,23 +931,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91323775-37AE-44DC-8259-7FCDE5D849E0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC650EC1-3E41-4FC6-BA6C-52921951A8DA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="220d4249-f262-4642-a86b-ff46de6e315d"/>
-    <ds:schemaRef ds:uri="965e701d-44ad-4371-a199-8fefe953808c"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>